<commit_message>
gladlab.mod and gladpath.run: nice and quick with best EULER_RATIO trend and overall values yet; 11sec a pop for 100 steps; correct direction for productivity
</commit_message>
<xml_diff>
--- a/ampl/output/aushistoric/agg-gladlab-knitro-0-aus-EPS_OUT_C_E_700-historic.xlsx
+++ b/ampl/output/aushistoric/agg-gladlab-knitro-0-aus-EPS_OUT_C_E_700-historic.xlsx
@@ -184,16 +184,16 @@
         <v>19</v>
       </c>
       <c r="D2" t="n">
-        <v>57.758030736363224</v>
+        <v>58.863157279110631</v>
       </c>
       <c r="E2" t="n">
-        <v>35.869840871298841</v>
+        <v>36.845950650053922</v>
       </c>
       <c r="F2" t="n">
-        <v>6.8788517479273104</v>
+        <v>6.665623311424171</v>
       </c>
       <c r="G2" t="n">
-        <v>7.082731429892041</v>
+        <v>7.2936368076005813</v>
       </c>
     </row>
     <row r="3">
@@ -204,19 +204,19 @@
         <v>1</v>
       </c>
       <c r="C3" t="n">
-        <v>20.233441849152058</v>
+        <v>20.279732331511337</v>
       </c>
       <c r="D3" t="n">
-        <v>59.414432750422868</v>
+        <v>60.565558015294819</v>
       </c>
       <c r="E3" t="n">
-        <v>36.907806725004598</v>
+        <v>37.919500238669535</v>
       </c>
       <c r="F3" t="n">
-        <v>7.0573680094480622</v>
+        <v>6.841561472747026</v>
       </c>
       <c r="G3" t="n">
-        <v>7.3023243284145085</v>
+        <v>7.52252212830129</v>
       </c>
     </row>
     <row r="4">
@@ -227,19 +227,19 @@
         <v>2</v>
       </c>
       <c r="C4" t="n">
-        <v>21.538012664856144</v>
+        <v>21.631144666991737</v>
       </c>
       <c r="D4" t="n">
-        <v>60.996134497878401</v>
+        <v>62.190400841368124</v>
       </c>
       <c r="E4" t="n">
-        <v>37.910610697235533</v>
+        <v>38.956202886293738</v>
       </c>
       <c r="F4" t="n">
-        <v>7.2309104470322865</v>
+        <v>7.0124312008383649</v>
       </c>
       <c r="G4" t="n">
-        <v>7.5073630515437975</v>
+        <v>7.7361091843479324</v>
       </c>
     </row>
     <row r="5">
@@ -250,19 +250,19 @@
         <v>3</v>
       </c>
       <c r="C5" t="n">
-        <v>22.902225961318393</v>
+        <v>23.042556531441296</v>
       </c>
       <c r="D5" t="n">
-        <v>62.519292941788606</v>
+        <v>63.754537013726427</v>
       </c>
       <c r="E5" t="n">
-        <v>38.883936550783538</v>
+        <v>39.962060168256372</v>
       </c>
       <c r="F5" t="n">
-        <v>7.4008003232070472</v>
+        <v>7.1795570707463536</v>
       </c>
       <c r="G5" t="n">
-        <v>7.7015651835335612</v>
+        <v>7.9382922884743081</v>
       </c>
     </row>
     <row r="6">
@@ -273,19 +273,19 @@
         <v>4</v>
       </c>
       <c r="C6" t="n">
-        <v>24.315909768382774</v>
+        <v>24.503753020465748</v>
       </c>
       <c r="D6" t="n">
-        <v>63.996929164756509</v>
+        <v>65.271540185411695</v>
       </c>
       <c r="E6" t="n">
-        <v>39.832477232972501</v>
+        <v>40.941993680366167</v>
       </c>
       <c r="F6" t="n">
-        <v>7.5680417822921822</v>
+        <v>7.3439464746892522</v>
       </c>
       <c r="G6" t="n">
-        <v>7.8875900364606961</v>
+        <v>8.1318554209312417</v>
       </c>
     </row>
     <row r="7">
@@ -296,19 +296,19 @@
         <v>5</v>
       </c>
       <c r="C7" t="n">
-        <v>25.771200524248332</v>
+        <v>26.007006265670462</v>
       </c>
       <c r="D7" t="n">
-        <v>65.439035800790393</v>
+        <v>66.751587174717244</v>
       </c>
       <c r="E7" t="n">
-        <v>40.760481132624783</v>
+        <v>41.90059747129159</v>
       </c>
       <c r="F7" t="n">
-        <v>7.7334072241814171</v>
+        <v>7.5063724242621817</v>
       </c>
       <c r="G7" t="n">
-        <v>8.0674667145142607</v>
+        <v>8.3189604693191903</v>
       </c>
     </row>
     <row r="8">
@@ -319,19 +319,19 @@
         <v>6</v>
       </c>
       <c r="C8" t="n">
-        <v>27.261196444768885</v>
+        <v>27.545001480293497</v>
       </c>
       <c r="D8" t="n">
-        <v>66.853145906319824</v>
+        <v>68.202618706954226</v>
       </c>
       <c r="E8" t="n">
-        <v>41.671927825023289</v>
+        <v>42.841961775620618</v>
       </c>
       <c r="F8" t="n">
-        <v>7.89750357521556</v>
+        <v>7.6674474719427419</v>
       </c>
       <c r="G8" t="n">
-        <v>8.2428102018865044</v>
+        <v>8.5012843503935649</v>
       </c>
     </row>
     <row r="9">
@@ -342,19 +342,19 @@
         <v>7</v>
       </c>
       <c r="C9" t="n">
-        <v>28.778678292547777</v>
+        <v>29.110466503821311</v>
       </c>
       <c r="D9" t="n">
-        <v>68.245852047187668</v>
+        <v>69.631481651404854</v>
       </c>
       <c r="E9" t="n">
-        <v>42.570077881675758</v>
+        <v>43.769547954154461</v>
       </c>
       <c r="F9" t="n">
-        <v>8.0608342422033488</v>
+        <v>7.8276800063556848</v>
       </c>
       <c r="G9" t="n">
-        <v>8.4148106491041066</v>
+        <v>8.6800831550632171</v>
       </c>
     </row>
     <row r="10">
@@ -365,19 +365,19 @@
         <v>8</v>
       </c>
       <c r="C10" t="n">
-        <v>30.31725354153404</v>
+        <v>30.696811037050377</v>
       </c>
       <c r="D10" t="n">
-        <v>69.622566261487677</v>
+        <v>71.043777300108133</v>
       </c>
       <c r="E10" t="n">
-        <v>43.457738357867669</v>
+        <v>44.686204637715946</v>
       </c>
       <c r="F10" t="n">
-        <v>8.2238145149556949</v>
+        <v>7.9874866319333053</v>
       </c>
       <c r="G10" t="n">
-        <v>8.5843912448062163</v>
+        <v>8.8563086916631537</v>
       </c>
     </row>
     <row r="11">
@@ -388,19 +388,19 @@
         <v>9</v>
       </c>
       <c r="C11" t="n">
-        <v>31.871406692484729</v>
+        <v>32.298613831785993</v>
       </c>
       <c r="D11" t="n">
-        <v>70.987814720582207</v>
+        <v>72.444219092942632</v>
       </c>
       <c r="E11" t="n">
-        <v>44.337182342248205</v>
+        <v>45.594386442604254</v>
       </c>
       <c r="F11" t="n">
-        <v>8.3867867660151898</v>
+        <v>8.147216169298142</v>
       </c>
       <c r="G11" t="n">
-        <v>8.7522461660813295</v>
+        <v>9.0307103663276997</v>
       </c>
     </row>
     <row r="12">
@@ -411,19 +411,19 @@
         <v>10</v>
       </c>
       <c r="C12" t="n">
-        <v>33.436972870297609</v>
+        <v>33.911597744950704</v>
       </c>
       <c r="D12" t="n">
-        <v>72.345490296999714</v>
+        <v>73.836815477401558</v>
       </c>
       <c r="E12" t="n">
-        <v>45.210746407297762</v>
+        <v>46.496529773505316</v>
       </c>
       <c r="F12" t="n">
-        <v>8.5500548949001516</v>
+        <v>8.3071759433109058</v>
       </c>
       <c r="G12" t="n">
-        <v>8.9190171972456156</v>
+        <v>9.2039628513025189</v>
       </c>
     </row>
     <row r="13">
@@ -434,19 +434,19 @@
         <v>11</v>
       </c>
       <c r="C13" t="n">
-        <v>35.009989005083412</v>
+        <v>35.531681905895063</v>
       </c>
       <c r="D13" t="n">
-        <v>73.698787733408352</v>
+        <v>75.224843648745107</v>
       </c>
       <c r="E13" t="n">
-        <v>46.080307305193145</v>
+        <v>47.394539789643041</v>
       </c>
       <c r="F13" t="n">
-        <v>8.7138752653381637</v>
+        <v>8.4676226144375679</v>
       </c>
       <c r="G13" t="n">
-        <v>9.0851849697801139</v>
+        <v>9.3765580895603016</v>
       </c>
     </row>
     <row r="14">
@@ -457,19 +457,19 @@
         <v>12</v>
       </c>
       <c r="C14" t="n">
-        <v>36.587160503604743</v>
+        <v>37.15558874763726</v>
       </c>
       <c r="D14" t="n">
-        <v>75.050433314510286</v>
+        <v>76.611134208695702</v>
       </c>
       <c r="E14" t="n">
-        <v>46.947478476361646</v>
+        <v>48.290073986854971</v>
       </c>
       <c r="F14" t="n">
-        <v>8.8784698674782909</v>
+        <v>8.6287797697852948</v>
       </c>
       <c r="G14" t="n">
-        <v>9.2511368675693451</v>
+        <v>9.5488999901433527</v>
       </c>
     </row>
     <row r="15">
@@ -480,19 +480,19 @@
         <v>13</v>
       </c>
       <c r="C15" t="n">
-        <v>38.165876361007669</v>
+        <v>38.780777306534453</v>
       </c>
       <c r="D15" t="n">
-        <v>76.402822246031747</v>
+        <v>77.998250048288412</v>
       </c>
       <c r="E15" t="n">
-        <v>47.813644021241942</v>
+        <v>49.18437530957339</v>
       </c>
       <c r="F15" t="n">
-        <v>9.0440359416861629</v>
+        <v>8.7908463570459965</v>
       </c>
       <c r="G15" t="n">
-        <v>9.4171871898506971</v>
+        <v>9.7212820683025996</v>
       </c>
     </row>
     <row r="16">
@@ -503,19 +503,19 @@
         <v>14</v>
       </c>
       <c r="C16" t="n">
-        <v>39.744223583580357</v>
+        <v>40.405855507169257</v>
       </c>
       <c r="D16" t="n">
-        <v>77.758292310710218</v>
+        <v>79.38880695168568</v>
       </c>
       <c r="E16" t="n">
-        <v>48.679542356849275</v>
+        <v>50.078634463351506</v>
       </c>
       <c r="F16" t="n">
-        <v>9.2107449735603755</v>
+        <v>8.9539983897521278</v>
       </c>
       <c r="G16" t="n">
-        <v>9.5835204830257652</v>
+        <v>9.8940080244594846</v>
       </c>
     </row>
     <row r="17">
@@ -526,19 +526,19 @@
         <v>15</v>
       </c>
       <c r="C17" t="n">
-        <v>41.321964393904729</v>
+        <v>42.030311237258971</v>
       </c>
       <c r="D17" t="n">
-        <v>79.119611178434809</v>
+        <v>80.785661468166381</v>
       </c>
       <c r="E17" t="n">
-        <v>49.546388447964937</v>
+        <v>50.973734564122807</v>
       </c>
       <c r="F17" t="n">
-        <v>9.3787639675728585</v>
+        <v>9.1184042569142054</v>
       </c>
       <c r="G17" t="n">
-        <v>9.7504656904984071</v>
+        <v>10.067340704807739</v>
       </c>
     </row>
     <row r="18">
@@ -549,19 +549,19 @@
         <v>16</v>
       </c>
       <c r="C18" t="n">
-        <v>42.89930230342032</v>
+        <v>43.654814574371926</v>
       </c>
       <c r="D18" t="n">
-        <v>80.489296109447793</v>
+        <v>82.191451412799594</v>
       </c>
       <c r="E18" t="n">
-        <v>50.416311654287775</v>
+        <v>51.872657848600575</v>
       </c>
       <c r="F18" t="n">
-        <v>9.5482605211436606</v>
+        <v>9.2842395837226999</v>
       </c>
       <c r="G18" t="n">
-        <v>9.9185013967098072</v>
+        <v>10.24193334743433</v>
       </c>
     </row>
     <row r="19">
@@ -572,19 +572,19 @@
         <v>17</v>
       </c>
       <c r="C19" t="n">
-        <v>44.475257169066722</v>
+        <v>45.277576690455781</v>
       </c>
       <c r="D19" t="n">
-        <v>81.868976307918601</v>
+        <v>83.607439353880082</v>
       </c>
       <c r="E19" t="n">
-        <v>51.290411129032009</v>
+        <v>52.775951636882773</v>
       </c>
       <c r="F19" t="n">
-        <v>9.7193764582733913</v>
+        <v>9.451640755597996</v>
       </c>
       <c r="G19" t="n">
-        <v>10.087847415696137</v>
+        <v>10.417872899436519</v>
       </c>
     </row>
     <row r="20">
@@ -595,19 +595,19 @@
         <v>18</v>
       </c>
       <c r="C20" t="n">
-        <v>46.049099489529141</v>
+        <v>46.897907316390636</v>
       </c>
       <c r="D20" t="n">
-        <v>83.25996737381152</v>
+        <v>85.035016922010172</v>
       </c>
       <c r="E20" t="n">
-        <v>52.169740974618293</v>
+        <v>53.684509351585845</v>
       </c>
       <c r="F20" t="n">
-        <v>9.8922437518308364</v>
+        <v>9.6207387993103239</v>
       </c>
       <c r="G20" t="n">
-        <v>10.258705612301059</v>
+        <v>10.595334123892654</v>
       </c>
     </row>
     <row r="21">
@@ -618,19 +618,19 @@
         <v>19</v>
       </c>
       <c r="C21" t="n">
-        <v>47.620162186714971</v>
+        <v>48.515463486246212</v>
       </c>
       <c r="D21" t="n">
-        <v>84.663315228268274</v>
+        <v>86.475301826012554</v>
       </c>
       <c r="E21" t="n">
-        <v>53.054945921258422</v>
+        <v>54.599418087716721</v>
       </c>
       <c r="F21" t="n">
-        <v>10.066979616224097</v>
+        <v>9.7916565280268255</v>
       </c>
       <c r="G21" t="n">
-        <v>10.43118155786836</v>
+        <v>10.774514154836197</v>
       </c>
     </row>
     <row r="22">
@@ -641,19 +641,19 @@
         <v>20</v>
       </c>
       <c r="C22" t="n">
-        <v>49.188231620795371</v>
+        <v>50.129751399488157</v>
       </c>
       <c r="D22" t="n">
-        <v>86.079948738003452</v>
+        <v>87.929157068510548</v>
       </c>
       <c r="E22" t="n">
-        <v>53.946887579473952</v>
+        <v>55.521137325599859</v>
       </c>
       <c r="F22" t="n">
-        <v>10.243695407818723</v>
+        <v>9.9645004606997389</v>
       </c>
       <c r="G22" t="n">
-        <v>10.605422153317255</v>
+        <v>10.955473395896638</v>
       </c>
     </row>
     <row r="23">
@@ -664,19 +664,19 @@
         <v>21</v>
       </c>
       <c r="C23" t="n">
-        <v>50.753067661313672</v>
+        <v>51.740826581327248</v>
       </c>
       <c r="D23" t="n">
-        <v>87.510633123240751</v>
+        <v>89.39746776040333</v>
       </c>
       <c r="E23" t="n">
-        <v>54.846000772654676</v>
+        <v>56.450453277948313</v>
       </c>
       <c r="F23" t="n">
-        <v>10.422490250180994</v>
+        <v>10.139373459435731</v>
       </c>
       <c r="G23" t="n">
-        <v>10.781482703740149</v>
+        <v>11.1383454324612</v>
       </c>
     </row>
     <row r="24">
@@ -687,19 +687,19 @@
         <v>22</v>
       </c>
       <c r="C24" t="n">
-        <v>52.314854770905697</v>
+        <v>53.348731111284692</v>
       </c>
       <c r="D24" t="n">
-        <v>88.956134130288675</v>
+        <v>90.880931229848287</v>
       </c>
       <c r="E24" t="n">
-        <v>55.752994152765176</v>
+        <v>57.387963581838676</v>
       </c>
       <c r="F24" t="n">
-        <v>10.603460627788099</v>
+        <v>10.316369310173837</v>
       </c>
       <c r="G24" t="n">
-        <v>10.959479280430578</v>
+        <v>11.32321894860201</v>
       </c>
     </row>
     <row r="25">
@@ -710,19 +710,19 @@
         <v>23</v>
       </c>
       <c r="C25" t="n">
-        <v>53.873733924059046</v>
+        <v>54.953610464111556</v>
       </c>
       <c r="D25" t="n">
-        <v>90.41706210044714</v>
+        <v>92.380182228069529</v>
       </c>
       <c r="E25" t="n">
-        <v>56.668372433195778</v>
+        <v>58.334169068235866</v>
       </c>
       <c r="F25" t="n">
-        <v>10.786694275598981</v>
+        <v>10.495575077840536</v>
       </c>
       <c r="G25" t="n">
-        <v>11.139481799785026</v>
+        <v>11.510164192242536</v>
       </c>
     </row>
     <row r="26">
@@ -733,19 +733,19 @@
         <v>24</v>
       </c>
       <c r="C26" t="n">
-        <v>55.429960290686552</v>
+        <v>56.555752636572059</v>
       </c>
       <c r="D26" t="n">
-        <v>91.893998882985926</v>
+        <v>93.895841240956003</v>
       </c>
       <c r="E26" t="n">
-        <v>57.592589735067122</v>
+        <v>59.289547494242029</v>
       </c>
       <c r="F26" t="n">
-        <v>10.97227351347926</v>
+        <v>10.677073135132339</v>
       </c>
       <c r="G26" t="n">
-        <v>11.321553167073434</v>
+        <v>11.699250943470465</v>
       </c>
     </row>
     <row r="27">
@@ -756,19 +756,19 @@
         <v>25</v>
       </c>
       <c r="C27" t="n">
-        <v>56.983902642990067</v>
+        <v>58.155555805443221</v>
       </c>
       <c r="D27" t="n">
-        <v>93.387517253674289</v>
+        <v>95.428528169529699</v>
       </c>
       <c r="E27" t="n">
-        <v>58.526079715677241</v>
+        <v>60.25452741095782</v>
       </c>
       <c r="F27" t="n">
-        <v>11.160276700604491</v>
+        <v>10.860941784902273</v>
       </c>
       <c r="G27" t="n">
-        <v>11.5057562520534</v>
+        <v>11.890543417636211</v>
       </c>
     </row>
     <row r="28">
@@ -779,19 +779,19 @@
         <v>26</v>
       </c>
       <c r="C28" t="n">
-        <v>58.536019551219724</v>
+        <v>59.753545697630791</v>
       </c>
       <c r="D28" t="n">
-        <v>94.898184718292825</v>
+        <v>96.978880993182187</v>
       </c>
       <c r="E28" t="n">
-        <v>59.469249914900516</v>
+        <v>61.22953157837123</v>
       </c>
       <c r="F28" t="n">
-        <v>11.350778917334637</v>
+        <v>11.047256622682072</v>
       </c>
       <c r="G28" t="n">
-        <v>11.692152356721177</v>
+        <v>12.084110228984505</v>
       </c>
     </row>
     <row r="29">
@@ -802,19 +802,19 @@
         <v>27</v>
       </c>
       <c r="C29" t="n">
-        <v>60.086852642710973</v>
+        <v>61.350351391114337</v>
       </c>
       <c r="D29" t="n">
-        <v>96.426571459782465</v>
+        <v>98.547524115250582</v>
       </c>
       <c r="E29" t="n">
-        <v>60.422489463364002</v>
+        <v>62.215022491061845</v>
       </c>
       <c r="F29" t="n">
-        <v>11.543852739196042</v>
+        <v>11.236091362053845</v>
       </c>
       <c r="G29" t="n">
-        <v>11.88080290801952</v>
+        <v>12.280030631246264</v>
       </c>
     </row>
     <row r="30">
@@ -825,19 +825,19 @@
         <v>28</v>
       </c>
       <c r="C30" t="n">
-        <v>61.637019354369386</v>
+        <v>62.946615627106937</v>
       </c>
       <c r="D30" t="n">
-        <v>97.97324769593439</v>
+        <v>100.13503428105145</v>
       </c>
       <c r="E30" t="n">
-        <v>61.386186963357332</v>
+        <v>63.211423110684379</v>
       </c>
       <c r="F30" t="n">
-        <v>11.739568930217841</v>
+        <v>11.427517163571173</v>
       </c>
       <c r="G30" t="n">
-        <v>12.071772443542857</v>
+        <v>12.478375604643498</v>
       </c>
     </row>
     <row r="31">
@@ -848,19 +848,19 @@
         <v>29</v>
       </c>
       <c r="C31" t="n">
-        <v>63.187186490656508</v>
+        <v>64.543000807716211</v>
       </c>
       <c r="D31" t="n">
-        <v>99.538766412024259</v>
+        <v>101.74196089480613</v>
       </c>
       <c r="E31" t="n">
-        <v>62.360733848024132</v>
+        <v>64.219122100887617</v>
       </c>
       <c r="F31" t="n">
-        <v>11.937996708021357</v>
+        <v>11.621603051146856</v>
       </c>
       <c r="G31" t="n">
-        <v>12.26512760258165</v>
+        <v>12.679210026227247</v>
       </c>
     </row>
     <row r="32">
@@ -871,19 +871,19 @@
         <v>30</v>
       </c>
       <c r="C32" t="n">
-        <v>64.738036629723055</v>
+        <v>66.140199491674451</v>
       </c>
       <c r="D32" t="n">
-        <v>101.12365294338512</v>
+        <v>103.36884035338031</v>
       </c>
       <c r="E32" t="n">
-        <v>63.346500217907476</v>
+        <v>65.238491980850355</v>
       </c>
       <c r="F32" t="n">
-        <v>12.139203635845266</v>
+        <v>11.818416445072112</v>
       </c>
       <c r="G32" t="n">
-        <v>12.460931164400739</v>
+        <v>12.882597109165459</v>
       </c>
     </row>
     <row r="33">
@@ -894,19 +894,19 @@
         <v>31</v>
       </c>
       <c r="C33" t="n">
-        <v>66.290265246905037</v>
+        <v>67.738929791334144</v>
       </c>
       <c r="D33" t="n">
-        <v>102.72841323570458</v>
+        <v>105.01619867224758</v>
       </c>
       <c r="E33" t="n">
-        <v>64.343835355990564</v>
+        <v>66.269893278086471</v>
       </c>
       <c r="F33" t="n">
-        <v>12.343255883689018</v>
+        <v>12.018023455871953</v>
       </c>
       <c r="G33" t="n">
-        <v>12.659242481158447</v>
+        <v>13.088599114247161</v>
       </c>
     </row>
     <row r="34">
@@ -917,19 +917,19 @@
         <v>32</v>
       </c>
       <c r="C34" t="n">
-        <v>67.844582991644856</v>
+        <v>69.339929285228919</v>
       </c>
       <c r="D34" t="n">
-        <v>104.35354185005947</v>
+        <v>106.68455234085245</v>
       </c>
       <c r="E34" t="n">
-        <v>65.353075047319862</v>
+        <v>67.313675829106842</v>
       </c>
       <c r="F34" t="n">
-        <v>12.550218548626503</v>
+        <v>12.220489119439383</v>
       </c>
       <c r="G34" t="n">
-        <v>12.860119298618351</v>
+        <v>13.297277397866573</v>
       </c>
     </row>
     <row r="35">
@@ -940,19 +940,19 @@
         <v>33</v>
       </c>
       <c r="C35" t="n">
-        <v>69.401713855583736</v>
+        <v>70.943950220940962</v>
       </c>
       <c r="D35" t="n">
-        <v>105.99952447274194</v>
+        <v>108.37440951659497</v>
       </c>
       <c r="E35" t="n">
-        <v>66.374545834302566</v>
+        <v>68.37018021783274</v>
       </c>
       <c r="F35" t="n">
-        <v>12.760155875375775</v>
+        <v>12.425877684651203</v>
       </c>
       <c r="G35" t="n">
-        <v>13.063618529218713</v>
+        <v>13.508692639489848</v>
       </c>
     </row>
     <row r="36">
@@ -963,19 +963,19 @@
         <v>34</v>
       </c>
       <c r="C36" t="n">
-        <v>70.962390852764841</v>
+        <v>72.551755009272981</v>
       </c>
       <c r="D36" t="n">
-        <v>107.66683973691428</v>
+        <v>110.08626959832813</v>
       </c>
       <c r="E36" t="n">
-        <v>67.408565719219524</v>
+        <v>69.439739531714935</v>
       </c>
       <c r="F36" t="n">
-        <v>12.973131446871873</v>
+        <v>12.6342527078952</v>
       </c>
       <c r="G36" t="n">
-        <v>13.269796384499756</v>
+        <v>13.72290458401892</v>
       </c>
     </row>
     <row r="37">
@@ -986,19 +986,19 @@
         <v>35</v>
       </c>
       <c r="C37" t="n">
-        <v>72.527353217833905</v>
+        <v>74.164110762710308</v>
       </c>
       <c r="D37" t="n">
-        <v>109.35595969196009</v>
+        <v>111.82062510139724</v>
       </c>
       <c r="E37" t="n">
-        <v>68.455445773827236</v>
+        <v>70.522679566738105</v>
       </c>
       <c r="F37" t="n">
-        <v>13.189208338185113</v>
+        <v>12.8456772462948</v>
       </c>
       <c r="G37" t="n">
-        <v>13.478708479269669</v>
+        <v>13.939972430734766</v>
       </c>
     </row>
     <row r="38">
@@ -1009,19 +1009,19 @@
         <v>36</v>
       </c>
       <c r="C38" t="n">
-        <v>74.097343449399261</v>
+        <v>75.781785637178629</v>
       </c>
       <c r="D38" t="n">
-        <v>111.06735070967254</v>
+        <v>113.5779615878612</v>
       </c>
       <c r="E38" t="n">
-        <v>69.51549102014495</v>
+        <v>71.619319370238145</v>
       </c>
       <c r="F38" t="n">
-        <v>13.40844927018126</v>
+        <v>13.060213879940131</v>
       </c>
       <c r="G38" t="n">
-        <v>13.690409944490517</v>
+        <v>14.159954644879116</v>
       </c>
     </row>
     <row r="39">
@@ -1032,19 +1032,19 @@
         <v>37</v>
       </c>
       <c r="C39" t="n">
-        <v>75.673104697281488</v>
+        <v>77.405546890237616</v>
       </c>
       <c r="D39" t="n">
-        <v>112.80147397107864</v>
+        <v>115.35875869036052</v>
       </c>
       <c r="E39" t="n">
-        <v>70.589001385440227</v>
+        <v>72.729972063923654</v>
       </c>
       <c r="F39" t="n">
-        <v>13.630916695101165</v>
+        <v>13.277924830096042</v>
       </c>
       <c r="G39" t="n">
-        <v>13.904955425569616</v>
+        <v>14.382909069690713</v>
       </c>
     </row>
     <row r="40">
@@ -1055,19 +1055,19 @@
         <v>38</v>
       </c>
       <c r="C40" t="n">
-        <v>77.25537800852446</v>
+        <v>79.036159258115674</v>
       </c>
       <c r="D40" t="n">
-        <v>114.55878637374713</v>
+        <v>117.16349151550281</v>
       </c>
       <c r="E40" t="n">
-        <v>71.676272257271819</v>
+        <v>73.854945421662606</v>
       </c>
       <c r="F40" t="n">
-        <v>13.856672895944875</v>
+        <v>13.498872091867426</v>
       </c>
       <c r="G40" t="n">
-        <v>14.122399215783355</v>
+        <v>14.608893116959065</v>
       </c>
     </row>
     <row r="41">
@@ -1078,19 +1078,19 @@
         <v>39</v>
       </c>
       <c r="C41" t="n">
-        <v>78.844900091876411</v>
+        <v>80.67438385000851</v>
       </c>
       <c r="D41" t="n">
-        <v>116.33974053491085</v>
+        <v>118.99263041298792</v>
       </c>
       <c r="E41" t="n">
-        <v>72.777594914528493</v>
+        <v>74.994542781474408</v>
       </c>
       <c r="F41" t="n">
-        <v>14.085780002252257</v>
+        <v>13.723117506168856</v>
       </c>
       <c r="G41" t="n">
-        <v>14.342795122906358</v>
+        <v>14.837963564866888</v>
       </c>
     </row>
     <row r="42">
@@ -1101,19 +1101,19 @@
         <v>40</v>
       </c>
       <c r="C42" t="n">
-        <v>80.442402090671465</v>
+        <v>82.320977272714018</v>
       </c>
       <c r="D42" t="n">
-        <v>118.14478621999675</v>
+        <v>120.84664220463353</v>
       </c>
       <c r="E42" t="n">
-        <v>73.893256806363496</v>
+        <v>76.149063421651988</v>
       </c>
       <c r="F42" t="n">
-        <v>14.318300125629003</v>
+        <v>13.950722899493748</v>
       </c>
       <c r="G42" t="n">
-        <v>14.566196720556524</v>
+        <v>15.07017678154681</v>
       </c>
     </row>
     <row r="43">
@@ -1124,19 +1124,19 @@
         <v>41</v>
       </c>
       <c r="C43" t="n">
-        <v>82.048609053047997</v>
+        <v>83.97669146227301</v>
       </c>
       <c r="D43" t="n">
-        <v>119.97437051139724</v>
+        <v>122.72599047912794</v>
       </c>
       <c r="E43" t="n">
-        <v>75.023542100049781</v>
+        <v>77.318804530523352</v>
       </c>
       <c r="F43" t="n">
-        <v>14.554295408077264</v>
+        <v>14.181750237616596</v>
       </c>
       <c r="G43" t="n">
-        <v>14.79265723890223</v>
+        <v>15.305589250925026</v>
       </c>
     </row>
     <row r="44">
@@ -1147,19 +1147,19 @@
         <v>42</v>
       </c>
       <c r="C44" t="n">
-        <v>83.664239767169903</v>
+        <v>85.642271320619116</v>
       </c>
       <c r="D44" t="n">
-        <v>121.8289386778893</v>
+        <v>124.6311356469417</v>
       </c>
       <c r="E44" t="n">
-        <v>76.168732254053609</v>
+        <v>78.504062888119805</v>
       </c>
       <c r="F44" t="n">
-        <v>14.79382813886833</v>
+        <v>14.416261719354885</v>
       </c>
       <c r="G44" t="n">
-        <v>15.022229733892452</v>
+        <v>15.544257895735754</v>
       </c>
     </row>
     <row r="45">
@@ -1170,19 +1170,19 @@
         <v>43</v>
       </c>
       <c r="C45" t="n">
-        <v>85.290006724804329</v>
+        <v>87.318450116730219</v>
       </c>
       <c r="D45" t="n">
-        <v>123.70893437642449</v>
+        <v>126.56253647915848</v>
       </c>
       <c r="E45" t="n">
-        <v>77.329107312862789</v>
+        <v>79.705131014513242</v>
       </c>
       <c r="F45" t="n">
-        <v>15.036960841410211</v>
+        <v>14.654319653063185</v>
       </c>
       <c r="G45" t="n">
-        <v>15.25496731526883</v>
+        <v>15.786238847142425</v>
       </c>
     </row>
     <row r="46">
@@ -1193,19 +1193,19 @@
         <v>44</v>
       </c>
       <c r="C46" t="n">
-        <v>86.926614950495193</v>
+        <v>89.0059518145151</v>
       </c>
       <c r="D46" t="n">
-        <v>125.6148001278484</v>
+        <v>128.52065259520791</v>
       </c>
       <c r="E46" t="n">
-        <v>78.504947368370381</v>
+        <v>80.922299335898757</v>
       </c>
       <c r="F46" t="n">
-        <v>15.283756384657169</v>
+        <v>14.895986509390877</v>
       </c>
       <c r="G46" t="n">
-        <v>15.490923563402013</v>
+        <v>16.031587963363798</v>
       </c>
     </row>
     <row r="47">
@@ -1216,19 +1216,19 @@
         <v>45</v>
       </c>
       <c r="C47" t="n">
-        <v>88.574759031717434</v>
+        <v>90.705492448405636</v>
       </c>
       <c r="D47" t="n">
-        <v>127.54697678861393</v>
+        <v>130.50594452187667</v>
       </c>
       <c r="E47" t="n">
-        <v>79.696531564892481</v>
+        <v>82.155858090082276</v>
       </c>
       <c r="F47" t="n">
-        <v>15.534277904394862</v>
+        <v>15.141325010425097</v>
       </c>
       <c r="G47" t="n">
-        <v>15.73015188039618</v>
+        <v>16.280361251364493</v>
       </c>
     </row>
     <row r="48">
@@ -1239,19 +1239,19 @@
         <v>46</v>
       </c>
       <c r="C48" t="n">
-        <v>90.23512216303503</v>
+        <v>92.417779425695699</v>
       </c>
       <c r="D48" t="n">
-        <v>129.5059053423744</v>
+        <v>132.51887358635955</v>
       </c>
       <c r="E48" t="n">
-        <v>80.90413688887827</v>
+        <v>83.406097373998193</v>
       </c>
       <c r="F48" t="n">
-        <v>15.788588833118069</v>
+        <v>15.390398203451696</v>
       </c>
       <c r="G48" t="n">
-        <v>15.972705353132458</v>
+        <v>16.532614952786314</v>
       </c>
     </row>
     <row r="49">
@@ -1262,19 +1262,19 @@
         <v>47</v>
       </c>
       <c r="C49" t="n">
-        <v>91.90837779054705</v>
+        <v>94.1435108393066</v>
       </c>
       <c r="D49" t="n">
-        <v>131.49202807812898</v>
+        <v>134.55990188084252</v>
       </c>
       <c r="E49" t="n">
-        <v>82.128039220006002</v>
+        <v>84.673306623670001</v>
       </c>
       <c r="F49" t="n">
-        <v>16.046752947311848</v>
+        <v>15.643269518999672</v>
       </c>
       <c r="G49" t="n">
-        <v>16.218636981053766</v>
+        <v>16.788405434763831</v>
       </c>
     </row>
     <row r="50">
@@ -1285,19 +1285,19 @@
         <v>48</v>
       </c>
       <c r="C50" t="n">
-        <v>93.595190844797841</v>
+        <v>95.883375664519704</v>
       </c>
       <c r="D50" t="n">
-        <v>133.50578922713288</v>
+        <v>136.62949216116664</v>
       </c>
       <c r="E50" t="n">
-        <v>83.36851457268645</v>
+        <v>85.957774774425275</v>
       </c>
       <c r="F50" t="n">
-        <v>16.308834435151642</v>
+        <v>15.90000282251391</v>
       </c>
       <c r="G50" t="n">
-        <v>16.467999983599931</v>
+        <v>17.0477890608373</v>
       </c>
     </row>
     <row r="51">
@@ -1308,19 +1308,19 @@
         <v>49</v>
       </c>
       <c r="C51" t="n">
-        <v>95.296217881969042</v>
+        <v>97.638054247806764</v>
       </c>
       <c r="D51" t="n">
-        <v>135.54763497271614</v>
+        <v>138.72810860749183</v>
       </c>
       <c r="E51" t="n">
-        <v>84.625839384024943</v>
+        <v>87.259790947585884</v>
       </c>
       <c r="F51" t="n">
-        <v>16.574897942604515</v>
+        <v>16.160662503956647</v>
       </c>
       <c r="G51" t="n">
-        <v>16.720847849219652</v>
+        <v>17.31082242604927</v>
       </c>
     </row>
     <row r="52">
@@ -1331,19 +1331,19 @@
         <v>50</v>
       </c>
       <c r="C52" t="n">
-        <v>97.01210707638613</v>
+        <v>99.408218350523128</v>
       </c>
       <c r="D52" t="n">
-        <v>137.61801339168281</v>
+        <v>140.85621696556629</v>
       </c>
       <c r="E52" t="n">
-        <v>85.900290609619717</v>
+        <v>88.579644547579107</v>
       </c>
       <c r="F52" t="n">
-        <v>16.84500862760337</v>
+        <v>16.425313454085288</v>
       </c>
       <c r="G52" t="n">
-        <v>16.977234323112878</v>
+        <v>17.577562291627579</v>
       </c>
     </row>
     <row r="53">
@@ -1354,19 +1354,19 @@
         <v>51</v>
       </c>
       <c r="C53" t="n">
-        <v>98.743498295340103</v>
+        <v>101.19453151676103</v>
       </c>
       <c r="D53" t="n">
-        <v>139.71737473571278</v>
+        <v>143.01428493519606</v>
       </c>
       <c r="E53" t="n">
-        <v>87.192145605289994</v>
+        <v>89.917625535942022</v>
       </c>
       <c r="F53" t="n">
-        <v>17.119232181413867</v>
+        <v>16.694021050724505</v>
       </c>
       <c r="G53" t="n">
-        <v>17.237213392747709</v>
+        <v>17.848065602473447</v>
       </c>
     </row>
     <row r="54">
@@ -1377,19 +1377,19 @@
         <v>52</v>
       </c>
       <c r="C54" t="n">
-        <v>100.49102359858352</v>
+        <v>102.99764955925569</v>
       </c>
       <c r="D54" t="n">
-        <v>141.84617126195988</v>
+        <v>145.20278297315247</v>
       </c>
       <c r="E54" t="n">
-        <v>88.501682916168747</v>
+        <v>91.274024806997375</v>
       </c>
       <c r="F54" t="n">
-        <v>17.39763485986678</v>
+        <v>16.966851218875323</v>
       </c>
       <c r="G54" t="n">
-        <v>17.500839325540241</v>
+        <v>18.122389683729907</v>
       </c>
     </row>
     <row r="55">
@@ -1400,19 +1400,19 @@
         <v>53</v>
       </c>
       <c r="C55" t="n">
-        <v>102.25530706357935</v>
+        <v>104.81822089626536</v>
       </c>
       <c r="D55" t="n">
-        <v>144.0048575885956</v>
+        <v>147.42218415008372</v>
       </c>
       <c r="E55" t="n">
-        <v>89.82918183707045</v>
+        <v>92.649134271924126</v>
       </c>
       <c r="F55" t="n">
-        <v>17.680283495438157</v>
+        <v>17.243870434126077</v>
       </c>
       <c r="G55" t="n">
-        <v>17.768166623695993</v>
+        <v>18.400592056117961</v>
       </c>
     </row>
     <row r="56">
@@ -1423,19 +1423,19 @@
         <v>54</v>
       </c>
       <c r="C56" t="n">
-        <v>104.03696538263506</v>
+        <v>106.65688718688119</v>
       </c>
       <c r="D56" t="n">
-        <v>146.19389124690395</v>
+        <v>149.67296452204141</v>
       </c>
       <c r="E56" t="n">
-        <v>91.17492289110254</v>
+        <v>94.043247939755261</v>
       </c>
       <c r="F56" t="n">
-        <v>17.967245537018176</v>
+        <v>17.525145794419156</v>
       </c>
       <c r="G56" t="n">
-        <v>18.039250157848326</v>
+        <v>18.682730736227601</v>
       </c>
     </row>
     <row r="57">
@@ -1446,19 +1446,19 @@
         <v>55</v>
       </c>
       <c r="C57" t="n">
-        <v>105.83660819185393</v>
+        <v>108.51428280131687</v>
       </c>
       <c r="D57" t="n">
-        <v>148.41373251046139</v>
+        <v>151.95560327177262</v>
       </c>
       <c r="E57" t="n">
-        <v>92.539188054672834</v>
+        <v>95.456661229565313</v>
       </c>
       <c r="F57" t="n">
-        <v>18.258589052073113</v>
+        <v>17.810745066394677</v>
       </c>
       <c r="G57" t="n">
-        <v>18.314145066690152</v>
+        <v>18.968864083867778</v>
       </c>
     </row>
     <row r="58">
@@ -1469,19 +1469,19 @@
         <v>56</v>
       </c>
       <c r="C58" t="n">
-        <v>107.65483839448758</v>
+        <v>110.39103519448855</v>
       </c>
       <c r="D58" t="n">
-        <v>150.66484501999719</v>
+        <v>154.27058262165113</v>
       </c>
       <c r="E58" t="n">
-        <v>93.922260959593899</v>
+        <v>96.889671749339598</v>
       </c>
       <c r="F58" t="n">
-        <v>18.554382792038162</v>
+        <v>18.100736695855591</v>
       </c>
       <c r="G58" t="n">
-        <v>18.592906919063442</v>
+        <v>19.259050853186832</v>
       </c>
     </row>
     <row r="59">
@@ -1492,19 +1492,19 @@
         <v>57</v>
       </c>
       <c r="C59" t="n">
-        <v>109.4922523882982</v>
+        <v>112.2877646023272</v>
       </c>
       <c r="D59" t="n">
-        <v>152.94769563029774</v>
+        <v>156.61838830411617</v>
       </c>
       <c r="E59" t="n">
-        <v>95.324427149882055</v>
+        <v>98.342579053093971</v>
       </c>
       <c r="F59" t="n">
-        <v>18.854696196698981</v>
+        <v>18.395189856052401</v>
       </c>
       <c r="G59" t="n">
-        <v>18.875591652090048</v>
+        <v>19.553350268196748</v>
       </c>
     </row>
     <row r="60">
@@ -1515,19 +1515,19 @@
         <v>58</v>
       </c>
       <c r="C60" t="n">
-        <v>111.34944017575079</v>
+        <v>114.20508410919443</v>
       </c>
       <c r="D60" t="n">
-        <v>155.26275441667457</v>
+        <v>158.99950945572991</v>
       </c>
       <c r="E60" t="n">
-        <v>96.745974342466553</v>
+        <v>99.815684856608669</v>
       </c>
       <c r="F60" t="n">
-        <v>19.15959943038342</v>
+        <v>18.694174417301586</v>
       </c>
       <c r="G60" t="n">
-        <v>19.162255417773835</v>
+        <v>19.851821995113131</v>
       </c>
     </row>
     <row r="61">
@@ -1538,19 +1538,19 @@
         <v>59</v>
       </c>
       <c r="C61" t="n">
-        <v>113.22698545385873</v>
+        <v>116.14359965501185</v>
       </c>
       <c r="D61" t="n">
-        <v>157.61049624835414</v>
+        <v>161.41443894428701</v>
       </c>
       <c r="E61" t="n">
-        <v>98.187191786006068</v>
+        <v>101.30929288514223</v>
       </c>
       <c r="F61" t="n">
-        <v>19.469163412637446</v>
+        <v>18.997760940279456</v>
       </c>
       <c r="G61" t="n">
-        <v>19.452955701897633</v>
+        <v>20.154526184573541</v>
       </c>
     </row>
     <row r="62">
@@ -1561,19 +1561,19 @@
         <v>60</v>
       </c>
       <c r="C62" t="n">
-        <v>115.12546567240389</v>
+        <v>118.10391033388568</v>
       </c>
       <c r="D62" t="n">
-        <v>159.99139799238887</v>
+        <v>163.86367331925732</v>
       </c>
       <c r="E62" t="n">
-        <v>99.64837178150637</v>
+        <v>102.82370883321151</v>
       </c>
       <c r="F62" t="n">
-        <v>19.783459785095172</v>
+        <v>19.306020657799706</v>
       </c>
       <c r="G62" t="n">
-        <v>19.747749115542558</v>
+        <v>20.461523375159981</v>
       </c>
     </row>
     <row r="63">
@@ -1584,19 +1584,19 @@
         <v>61</v>
       </c>
       <c r="C63" t="n">
-        <v>117.04545226569971</v>
+        <v>120.08660892719632</v>
       </c>
       <c r="D63" t="n">
-        <v>162.40594135242179</v>
+        <v>166.3477137503597</v>
       </c>
       <c r="E63" t="n">
-        <v>101.12980824849885</v>
+        <v>104.35923994119227</v>
       </c>
       <c r="F63" t="n">
-        <v>20.10256094189587</v>
+        <v>19.619025541294036</v>
       </c>
       <c r="G63" t="n">
-        <v>20.04669355621737</v>
+        <v>20.77287457005599</v>
       </c>
     </row>
     <row r="64">
@@ -1607,19 +1607,19 @@
         <v>62</v>
       </c>
       <c r="C64" t="n">
-        <v>118.98751086606897</v>
+        <v>122.09228315851654</v>
       </c>
       <c r="D64" t="n">
-        <v>164.85461191482895</v>
+        <v>168.86706559478694</v>
       </c>
       <c r="E64" t="n">
-        <v>102.63179744227352</v>
+        <v>105.91619611125958</v>
       </c>
       <c r="F64" t="n">
-        <v>20.426540035999189</v>
+        <v>19.936848333349211</v>
       </c>
       <c r="G64" t="n">
-        <v>20.349847199603854</v>
+        <v>21.08864122757484</v>
       </c>
     </row>
     <row r="65">
@@ -1630,19 +1630,19 @@
         <v>63</v>
       </c>
       <c r="C65" t="n">
-        <v>120.95220171402141</v>
+        <v>124.12151588508868</v>
       </c>
       <c r="D65" t="n">
-        <v>167.33789956864402</v>
+        <v>171.4222391005745</v>
       </c>
       <c r="E65" t="n">
-        <v>104.15463782630961</v>
+        <v>107.49488949896748</v>
       </c>
       <c r="F65" t="n">
-        <v>20.755471006950653</v>
+        <v>20.259562628234221</v>
       </c>
       <c r="G65" t="n">
-        <v>20.65726870661139</v>
+        <v>21.408885356423671</v>
       </c>
     </row>
     <row r="66">
@@ -1653,19 +1653,19 @@
         <v>64</v>
       </c>
       <c r="C66" t="n">
-        <v>122.94008016311992</v>
+        <v>126.17488583743454</v>
       </c>
       <c r="D66" t="n">
-        <v>169.85629852773909</v>
+        <v>174.01374924687588</v>
       </c>
       <c r="E66" t="n">
-        <v>105.69863020562678</v>
+        <v>109.09563526010382</v>
       </c>
       <c r="F66" t="n">
-        <v>21.089428593116061</v>
+        <v>20.587242883743894</v>
       </c>
       <c r="G66" t="n">
-        <v>20.969017179649494</v>
+        <v>21.733669564507768</v>
       </c>
     </row>
     <row r="67">
@@ -1676,19 +1676,19 @@
         <v>65</v>
       </c>
       <c r="C67" t="n">
-        <v>124.95169721551179</v>
+        <v>128.25296762793812</v>
       </c>
       <c r="D67" t="n">
-        <v>172.41030779341796</v>
+        <v>176.64211583586831</v>
       </c>
       <c r="E67" t="n">
-        <v>107.26407785454424</v>
+        <v>110.71875157853187</v>
       </c>
       <c r="F67" t="n">
-        <v>21.428488392341578</v>
+        <v>20.91996444097672</v>
       </c>
       <c r="G67" t="n">
-        <v>21.285152269182991</v>
+        <v>22.063057097974323</v>
       </c>
     </row>
     <row r="68">
@@ -1699,19 +1699,19 @@
         <v>66</v>
       </c>
       <c r="C68" t="n">
-        <v>126.9876000146554</v>
+        <v>130.35633173942182</v>
       </c>
       <c r="D68" t="n">
-        <v>175.00043090755594</v>
+        <v>179.30786305422961</v>
       </c>
       <c r="E68" t="n">
-        <v>108.85128678261496</v>
+        <v>112.36455983671289</v>
       </c>
       <c r="F68" t="n">
-        <v>21.772726864519349</v>
+        <v>21.257803513053474</v>
       </c>
       <c r="G68" t="n">
-        <v>21.605734096517075</v>
+        <v>22.397111752039418</v>
       </c>
     </row>
     <row r="69">
@@ -1722,19 +1722,19 @@
         <v>67</v>
       </c>
       <c r="C69" t="n">
-        <v>129.04833217335317</v>
+        <v>132.4855443592424</v>
       </c>
       <c r="D69" t="n">
-        <v>177.62717676455364</v>
+        <v>182.01151957621019</v>
       </c>
       <c r="E69" t="n">
-        <v>110.46056583170304</v>
+        <v>114.03338462155979</v>
       </c>
       <c r="F69" t="n">
-        <v>22.122221399854787</v>
+        <v>21.600837226561726</v>
       </c>
       <c r="G69" t="n">
-        <v>21.930823493276716</v>
+        <v>22.73589795741049</v>
       </c>
     </row>
     <row r="70">
@@ -1745,19 +1745,19 @@
         <v>68</v>
       </c>
       <c r="C70" t="n">
-        <v>131.13443402263937</v>
+        <v>134.64116711006781</v>
       </c>
       <c r="D70" t="n">
-        <v>180.2910587496859</v>
+        <v>184.75361858914869</v>
       </c>
       <c r="E70" t="n">
-        <v>112.09222689419103</v>
+        <v>115.72555308977934</v>
       </c>
       <c r="F70" t="n">
-        <v>22.477050278620993</v>
+        <v>21.949143622789379</v>
       </c>
       <c r="G70" t="n">
-        <v>22.260481751868653</v>
+        <v>23.07948062809886</v>
       </c>
     </row>
     <row r="71">
@@ -1768,19 +1768,19 @@
         <v>69</v>
       </c>
       <c r="C71" t="n">
-        <v>133.24644272700695</v>
+        <v>136.82375764843334</v>
       </c>
       <c r="D71" t="n">
-        <v>182.99259512588117</v>
+        <v>187.53469831263118</v>
       </c>
       <c r="E71" t="n">
-        <v>113.74658495263685</v>
+        <v>117.44139425017244</v>
       </c>
       <c r="F71" t="n">
-        <v>22.83729270891083</v>
+        <v>22.302801633359586</v>
       </c>
       <c r="G71" t="n">
-        <v>22.594770741258873</v>
+        <v>23.427924901974137</v>
       </c>
     </row>
   </sheetData>

</xml_diff>